<commit_message>
add minor revision to graphs and scenarios
</commit_message>
<xml_diff>
--- a/arpascm/Data/File_HMI_Scenari_Limite_e_Critico_rev1.xlsx
+++ b/arpascm/Data/File_HMI_Scenari_Limite_e_Critico_rev1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego.pinto\PycharmProjects\ARPA-FCA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B6AB0-5194-438C-98AD-A576F8E35596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A59E45F-FCFD-4D2A-A61A-17A3A8B73E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="2100" windowWidth="23040" windowHeight="12204" xr2:uid="{9B66E39A-66B8-4875-96A8-60673378B278}"/>
+    <workbookView xWindow="3648" yWindow="2100" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{9B66E39A-66B8-4875-96A8-60673378B278}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario_Limite" sheetId="7" r:id="rId1"/>
@@ -510,11 +510,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,6 +561,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -882,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10115017-072A-4AE3-A90C-65AE09B20F8F}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -899,65 +902,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>100</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>95</v>
       </c>
-      <c r="C2" s="1">
-        <f>(B2-$A$2)/$A$2</f>
-        <v>-0.05</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="C2" s="18">
+        <f>ABS((B2-$A$2)/$A$2)*100</f>
+        <v>5</v>
+      </c>
+      <c r="D2" s="6">
         <v>100</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>100</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>20</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -970,7 +973,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,65 +989,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>100</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>91.6</v>
       </c>
-      <c r="C2" s="1">
-        <f>(B2-$A$2)/$A$2</f>
-        <v>-8.4000000000000061E-2</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="C2" s="19">
+        <f>ABS((B2-$A$2)/$A$2)*100</f>
+        <v>8.4000000000000057</v>
+      </c>
+      <c r="D2" s="6">
         <v>100</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>90</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>30</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1056,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F72F11B-BED8-4552-B38E-D7D3FC3C15BB}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,70 +1076,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>100</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>88.75</v>
       </c>
-      <c r="C2" s="1">
-        <f>(B2-$A$2)/$A$2</f>
-        <v>-0.1125</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="C2" s="18">
+        <f>ABS((B2-$A$2)/$A$2)*100</f>
+        <v>11.25</v>
+      </c>
+      <c r="D2" s="6">
         <v>100</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="10">
         <v>88</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>60</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K3" s="14"/>
+      <c r="K3" s="13"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>